<commit_message>
eelgrass_acreage obtained from annual monitoring reports by the Piscataqua Region Estuary Partnership
</commit_message>
<xml_diff>
--- a/data/ecological_response/eelgrass_acres.xlsx
+++ b/data/ecological_response/eelgrass_acres.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annab\Documents\Projects\MS_Solute_Budgets\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annab\Documents\Projects\GreatBay_BoxModel\data\ecological_response\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5FAF5E-10A3-49B2-BFB8-F56A5AF5381E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EE4011-173C-4246-80FC-3CFEFCBCAA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{737870FF-6F98-466D-92EC-C9AFD76A2973}"/>
+    <workbookView xWindow="39030" yWindow="3465" windowWidth="14400" windowHeight="7275" xr2:uid="{737870FF-6F98-466D-92EC-C9AFD76A2973}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,24 +34,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Eelgrass_Coverage_Acres</t>
+    <t>GB_ZM_acres</t>
   </si>
   <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>https://scholars.unh.edu/cgi/viewcontent.cgi?article=1440&amp;context=prep</t>
-  </si>
-  <si>
-    <t>https://scholars.unh.edu/cgi/viewcontent.cgi?article=1408&amp;context=prep</t>
-  </si>
-  <si>
-    <t>https://scholars.unh.edu/cgi/viewcontent.cgi?article=1357&amp;context=prep</t>
+    <t>GBE_ZM_acres</t>
   </si>
 </sst>
 </file>
@@ -87,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -107,9 +99,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -147,7 +139,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -253,7 +245,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -395,18 +387,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A9B386-21D8-406C-B4F9-5D58ADCE630F}">
-  <dimension ref="A1:C24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175C2583-364C-4155-AE3F-FB14A047D33E}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -424,195 +416,282 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>2019</v>
-      </c>
-      <c r="B2">
-        <v>1450.6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+        <v>2023</v>
+      </c>
+      <c r="B2" s="1">
+        <v>855.56</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1024.51</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2017</v>
-      </c>
-      <c r="B3">
-        <v>1362.4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+        <v>2022</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1393.12</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1606.74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2016</v>
-      </c>
-      <c r="B4">
-        <v>1489.9</v>
+        <v>2021</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1266.03</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1566.47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2015</v>
-      </c>
-      <c r="B5">
-        <v>1319</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
+        <v>2019</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1344.99</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1570.87</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>1466</v>
+        <v>2017</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1362.42</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1546.66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>2013</v>
-      </c>
-      <c r="B7">
-        <v>1266</v>
+        <v>2016</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1489.9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1688.71</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="B8">
-        <v>1599</v>
+        <v>1319</v>
+      </c>
+      <c r="C8">
+        <v>1493</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="B9">
-        <v>1624</v>
+        <v>1466</v>
+      </c>
+      <c r="C9">
+        <v>1620</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="B10">
-        <v>1722</v>
+        <v>1266</v>
+      </c>
+      <c r="C10">
+        <v>1448</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="B11">
-        <v>1701</v>
+        <v>1599</v>
+      </c>
+      <c r="C11">
+        <v>1813</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2008</v>
+        <v>2011</v>
       </c>
       <c r="B12">
-        <v>1395</v>
+        <v>1624</v>
+      </c>
+      <c r="C12">
+        <v>1836</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2007</v>
+        <v>2010</v>
       </c>
       <c r="B13">
-        <v>1245</v>
+        <v>1722</v>
+      </c>
+      <c r="C13">
+        <v>1895</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>2006</v>
+        <v>2009</v>
       </c>
       <c r="B14">
-        <v>1321</v>
+        <v>1701</v>
+      </c>
+      <c r="C14">
+        <v>1890</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>2005</v>
+        <v>2008</v>
       </c>
       <c r="B15">
-        <v>2175</v>
+        <v>1395</v>
+      </c>
+      <c r="C15">
+        <v>1619</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
+        <v>2007</v>
+      </c>
+      <c r="B16">
+        <v>1245</v>
+      </c>
+      <c r="C16">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2006</v>
+      </c>
+      <c r="B17">
+        <v>1321</v>
+      </c>
+      <c r="C17">
+        <v>1623</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>2005</v>
+      </c>
+      <c r="B18">
+        <v>2175</v>
+      </c>
+      <c r="C18">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
         <v>2004</v>
       </c>
-      <c r="B16">
+      <c r="B19">
         <v>2042</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17">
+      <c r="C19">
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
         <v>2003</v>
       </c>
-      <c r="B17">
+      <c r="B20">
         <v>1627</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18">
+      <c r="C20">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
         <v>2002</v>
       </c>
-      <c r="B18">
+      <c r="B21">
         <v>1795</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19">
+      <c r="C21">
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
         <v>2001</v>
       </c>
-      <c r="B19">
+      <c r="B22">
         <v>2392</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20">
+      <c r="C22">
+        <v>2735</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
         <v>2000</v>
       </c>
-      <c r="B20">
+      <c r="B23">
         <v>1945</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21">
+      <c r="C23">
+        <v>2285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
         <v>1999</v>
       </c>
-      <c r="B21">
+      <c r="B24">
         <v>2130</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22">
+      <c r="C24">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
         <v>1998</v>
       </c>
-      <c r="B22">
+      <c r="B25">
         <v>2398</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26">
         <v>1997</v>
       </c>
-      <c r="B23">
+      <c r="B26">
         <v>2305</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>1996</v>
       </c>
-      <c r="B24">
+      <c r="B27">
         <v>2503</v>
+      </c>
+      <c r="C27">
+        <v>2894</v>
       </c>
     </row>
   </sheetData>

</xml_diff>